<commit_message>
really ready for submission
</commit_message>
<xml_diff>
--- a/data/data_overview.xlsx
+++ b/data/data_overview.xlsx
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>PFV_ga_traj.txt</t>
-  </si>
-  <si>
     <t>data structure</t>
   </si>
   <si>
@@ -36,85 +33,46 @@
     <t>data points (599) x channels of interest (15) +  time column</t>
   </si>
   <si>
-    <t>PFV_ga_topo.txt</t>
-  </si>
-  <si>
-    <t>data points (599) x all channels (40) +  time column</t>
-  </si>
-  <si>
-    <t>averaged data points across all conditions / participants for all channels</t>
-  </si>
-  <si>
-    <t>averaged data points across all conditions / participants for ROI channels</t>
-  </si>
-  <si>
-    <t>P1_P3_traj.txt</t>
-  </si>
-  <si>
-    <t>N170_l_traj.txt</t>
-  </si>
-  <si>
-    <t>N170_r_traj.txt</t>
-  </si>
-  <si>
-    <t>amplitude, ID, time, condition as separate columns (150948 x 1)</t>
-  </si>
-  <si>
-    <t>P1/P3 averaged time course across ROI channels for each participant / condition</t>
-  </si>
-  <si>
-    <t>N170 left averaged time course across ROI channels for each participant / condition</t>
-  </si>
-  <si>
-    <t>N170 right averaged time course across ROI channels for each participant / condition</t>
-  </si>
-  <si>
-    <t>channel names and coordinates</t>
-  </si>
-  <si>
-    <t>EEG_chanlocs.txt</t>
-  </si>
-  <si>
-    <t>labels, type, theta, radius, X, Y, Z, sp_theta, sph_phi, sph_radius, urchan</t>
-  </si>
-  <si>
-    <t>s_XX_condition.txt</t>
-  </si>
-  <si>
-    <t>separated for each participant and each condition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data points (599) x channel (40) </t>
-  </si>
-  <si>
-    <t>P1_singl_trial_data.txt</t>
-  </si>
-  <si>
-    <t>N170_l_singl_trial_data.txt</t>
-  </si>
-  <si>
-    <t>N170_r_singl_trial_data.txt</t>
-  </si>
-  <si>
-    <t>P3_singl_trial_data.txt</t>
-  </si>
-  <si>
-    <t>columns for channels, ROI_GA, emotion, ID, Trial (10625 x 13)</t>
-  </si>
-  <si>
-    <t>columns for channels, ROI_GA, emotion, ID, Trial (10625 x 8)</t>
-  </si>
-  <si>
-    <t>P1 mean amplitude for each trial per participant / condition</t>
-  </si>
-  <si>
-    <t>P3 mean amplitude for each trial per participant / condition</t>
-  </si>
-  <si>
-    <t>N170 left mean amplitude for each trial per participant / condition</t>
-  </si>
-  <si>
-    <t>N170 right mean amplitude for each trial per participant / condition</t>
+    <t>qn_data</t>
+  </si>
+  <si>
+    <t>demographics, behavioral and brain measures</t>
+  </si>
+  <si>
+    <t>app_qn</t>
+  </si>
+  <si>
+    <t>PFV_emo_topo</t>
+  </si>
+  <si>
+    <t>PFV_emo_topo_cg</t>
+  </si>
+  <si>
+    <t>PFV_emo_topo_tg</t>
+  </si>
+  <si>
+    <t>erp_vis_data</t>
+  </si>
+  <si>
+    <t>averaged data points across controls for all channels</t>
+  </si>
+  <si>
+    <t>averaged data points across Zirkus Empathico group for all channels</t>
+  </si>
+  <si>
+    <t>each row contains one variable</t>
+  </si>
+  <si>
+    <t>fidelity measures and qualitative questions</t>
+  </si>
+  <si>
+    <t>All channels x time x emotion</t>
+  </si>
+  <si>
+    <t>For topographical plots</t>
+  </si>
+  <si>
+    <t>To visualize ERP trajectory over time</t>
   </si>
 </sst>
 </file>
@@ -449,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,131 +426,76 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>